<commit_message>
Comment Clarification and Inputs.txt revision
</commit_message>
<xml_diff>
--- a/src/files/helloworld.xlsx
+++ b/src/files/helloworld.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Node</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Neighboring Nodes</t>
-  </si>
-  <si>
-    <t>Obstructed (T/F)</t>
   </si>
   <si>
     <t>Time (s)</t>
@@ -489,7 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -512,19 +509,19 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -567,7 +564,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -718,10 +715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,348 +766,319 @@
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="b">
-        <v>0</v>
+      <c r="B2">
+        <v>118</v>
+      </c>
+      <c r="C2">
+        <v>68</v>
+      </c>
+      <c r="D2">
+        <v>107</v>
+      </c>
+      <c r="E2">
+        <v>132</v>
+      </c>
+      <c r="F2">
+        <v>119</v>
+      </c>
+      <c r="G2">
+        <v>97</v>
+      </c>
+      <c r="H2">
+        <v>196</v>
+      </c>
+      <c r="I2">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="B3">
+        <v>107</v>
+      </c>
+      <c r="C3">
+        <v>69</v>
+      </c>
+      <c r="D3">
+        <v>124</v>
+      </c>
+      <c r="E3">
         <v>118</v>
       </c>
-      <c r="C3">
-        <v>68</v>
-      </c>
-      <c r="D3">
-        <v>107</v>
-      </c>
-      <c r="E3">
-        <v>132</v>
-      </c>
       <c r="F3">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="G3">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H3">
-        <v>196</v>
+        <v>229</v>
       </c>
       <c r="I3">
-        <v>111</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C4">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D4">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E4">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F4">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="G4">
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="H4">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="I4">
-        <v>182</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C5">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="D5">
-        <v>127</v>
+        <v>79</v>
       </c>
       <c r="E5">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F5">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="G5">
-        <v>188</v>
+        <v>119</v>
       </c>
       <c r="H5">
-        <v>205</v>
+        <v>179</v>
       </c>
       <c r="I5">
-        <v>242</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
+        <v>132</v>
+      </c>
+      <c r="C6">
+        <v>92</v>
+      </c>
+      <c r="D6">
+        <v>74</v>
+      </c>
+      <c r="E6">
         <v>105</v>
       </c>
-      <c r="C6">
-        <v>86</v>
-      </c>
-      <c r="D6">
-        <v>79</v>
-      </c>
-      <c r="E6">
-        <v>107</v>
-      </c>
       <c r="F6">
-        <v>171</v>
+        <v>204</v>
       </c>
       <c r="G6">
-        <v>119</v>
+        <v>177</v>
       </c>
       <c r="H6">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="I6">
-        <v>181</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="C7">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D7">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="E7">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F7">
-        <v>204</v>
+        <v>87</v>
       </c>
       <c r="G7">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="H7">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="I7">
-        <v>285</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
+        <v>112</v>
+      </c>
+      <c r="C8">
         <v>102</v>
       </c>
-      <c r="C8">
+      <c r="D8">
+        <v>112</v>
+      </c>
+      <c r="E8">
         <v>97</v>
       </c>
-      <c r="D8">
-        <v>85</v>
-      </c>
-      <c r="E8">
-        <v>102</v>
-      </c>
       <c r="F8">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="G8">
-        <v>215</v>
+        <v>140</v>
       </c>
       <c r="H8">
         <v>207</v>
       </c>
       <c r="I8">
-        <v>273</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="C9">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D9">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="E9">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F9">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="G9">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="H9">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="I9">
-        <v>124</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C10">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D10">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E10">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F10">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G10">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="H10">
-        <v>229</v>
+        <v>191</v>
       </c>
       <c r="I10">
-        <v>235</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C11">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D11">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="E11">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="F11">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G11">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="H11">
-        <v>191</v>
+        <v>266</v>
       </c>
       <c r="I11">
-        <v>93</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C12">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D12">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="E12">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F12">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="G12">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="H12">
-        <v>266</v>
+        <v>199</v>
       </c>
       <c r="I12">
-        <v>149</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="C13">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="D13">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="E13">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G13">
-        <v>159</v>
+        <v>191</v>
       </c>
       <c r="H13">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="I13">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>74</v>
-      </c>
-      <c r="C14">
-        <v>132</v>
-      </c>
-      <c r="D14">
-        <v>74</v>
-      </c>
-      <c r="E14">
-        <v>68</v>
-      </c>
-      <c r="F14">
-        <v>99</v>
-      </c>
-      <c r="G14">
-        <v>191</v>
-      </c>
-      <c r="H14">
-        <v>206</v>
-      </c>
-      <c r="I14">
         <v>151</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="E3:E14">
+  <sortState ref="E2:E13">
     <sortCondition descending="1" ref="E3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>